<commit_message>
lift and project has numerical issues
</commit_message>
<xml_diff>
--- a/examples/PoolingContract/PoolingContract_results.xlsx
+++ b/examples/PoolingContract/PoolingContract_results.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2900" yWindow="660" windowWidth="28800" windowHeight="15940" tabRatio="500"/>
+    <workbookView xWindow="39660" yWindow="2780" windowWidth="27180" windowHeight="14440" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="branchAndBound" sheetId="2" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="25">
   <si>
     <t>LB</t>
   </si>
@@ -100,7 +100,7 @@
     <t>Algorithm=Lagrangean decomposition</t>
   </si>
   <si>
-    <t>&gt;20,000</t>
+    <t>&gt;10,000</t>
   </si>
 </sst>
 </file>
@@ -445,7 +445,7 @@
   <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -613,23 +613,23 @@
         <v>-1338.89</v>
       </c>
       <c r="D10" s="3">
-        <v>-1340.31</v>
+        <v>-1340.51</v>
       </c>
       <c r="E10" s="4">
         <f>(D10-C10)/D10</f>
-        <v>1.0594563944161018E-3</v>
+        <v>1.2084952741866087E-3</v>
       </c>
       <c r="F10" s="3" t="s">
         <v>24</v>
       </c>
       <c r="G10" s="3">
-        <v>18267</v>
+        <v>8103</v>
       </c>
       <c r="H10" s="3">
-        <v>1760</v>
+        <v>1711</v>
       </c>
       <c r="I10" s="3">
-        <v>969</v>
+        <v>381</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
@@ -640,23 +640,23 @@
         <v>-1338.89</v>
       </c>
       <c r="D11" s="3">
-        <v>-1344.53</v>
+        <v>-1350.16</v>
       </c>
       <c r="E11" s="4">
         <f>(D11-C11)/D11</f>
-        <v>4.1947743821260019E-3</v>
+        <v>8.3471588552467713E-3</v>
       </c>
       <c r="F11" s="3" t="s">
         <v>24</v>
       </c>
       <c r="G11" s="3">
-        <v>18799</v>
+        <v>9317</v>
       </c>
       <c r="H11" s="3">
-        <v>1300</v>
+        <v>809</v>
       </c>
       <c r="I11" s="3">
-        <v>103</v>
+        <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
@@ -667,23 +667,23 @@
         <v>-1338.72</v>
       </c>
       <c r="D12" s="3">
-        <v>-1354.57</v>
+        <v>-1356.72</v>
       </c>
       <c r="E12" s="4">
         <f>(D12-C12)/D12</f>
-        <v>1.1701130247975306E-2</v>
+        <v>1.3267291703520255E-2</v>
       </c>
       <c r="F12" s="3" t="s">
         <v>24</v>
       </c>
       <c r="G12" s="3">
-        <v>20005</v>
+        <v>10220</v>
       </c>
       <c r="H12" s="3">
-        <v>1073</v>
+        <v>1305</v>
       </c>
       <c r="I12" s="3">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
@@ -721,37 +721,76 @@
       <c r="B18" s="3">
         <v>3</v>
       </c>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
+      <c r="C18" s="3">
+        <v>-1338.68</v>
+      </c>
+      <c r="D18" s="3">
+        <v>-1341.93</v>
+      </c>
+      <c r="E18" s="4">
+        <f>(D18-C18)/D18</f>
+        <v>2.4218848971257812E-3</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G18" s="3">
+        <v>9924</v>
+      </c>
       <c r="H18" s="3"/>
-      <c r="I18" s="3"/>
+      <c r="I18" s="3">
+        <v>363</v>
+      </c>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B19" s="3">
         <v>9</v>
       </c>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="3"/>
+      <c r="C19" s="3">
+        <v>-1313.93</v>
+      </c>
+      <c r="D19" s="3">
+        <v>-1414.68</v>
+      </c>
+      <c r="E19" s="4">
+        <f>(D19-C19)/D19</f>
+        <v>7.1217519156275624E-2</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G19" s="3">
+        <v>10511</v>
+      </c>
       <c r="H19" s="3"/>
-      <c r="I19" s="3"/>
+      <c r="I19" s="3">
+        <v>43</v>
+      </c>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B20" s="3">
         <v>27</v>
       </c>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="3"/>
-      <c r="G20" s="3"/>
+      <c r="C20" s="3">
+        <v>-1308.9100000000001</v>
+      </c>
+      <c r="D20" s="3">
+        <v>-1491.52</v>
+      </c>
+      <c r="E20" s="4">
+        <f>(D20-C20)/D20</f>
+        <v>0.12243214975327177</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G20" s="3">
+        <v>10893</v>
+      </c>
       <c r="H20" s="3"/>
-      <c r="I20" s="3"/>
+      <c r="I20" s="3">
+        <v>9</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
test all the examples
</commit_message>
<xml_diff>
--- a/examples/PoolingContract/PoolingContract_results.xlsx
+++ b/examples/PoolingContract/PoolingContract_results.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="39660" yWindow="2780" windowWidth="27180" windowHeight="14440" tabRatio="500"/>
+    <workbookView xWindow="38940" yWindow="2240" windowWidth="27180" windowHeight="14440" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="branchAndBound" sheetId="2" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="27">
   <si>
     <t>LB</t>
   </si>
@@ -101,6 +101,12 @@
   </si>
   <si>
     <t>&gt;10,000</t>
+  </si>
+  <si>
+    <t>Solver=Antigone</t>
+  </si>
+  <si>
+    <t>Solver=SCIP</t>
   </si>
 </sst>
 </file>
@@ -158,13 +164,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -444,7 +451,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
       <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
@@ -799,10 +806,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -843,14 +850,14 @@
         <v>3</v>
       </c>
       <c r="C2">
-        <v>-1338.89</v>
+        <v>-1338.24</v>
       </c>
       <c r="D2">
-        <v>-1340.23</v>
+        <v>-1338.24</v>
       </c>
       <c r="E2" s="2">
         <f>-(C2-D2)/D2</f>
-        <v>9.9982838766474267E-4</v>
+        <v>0</v>
       </c>
       <c r="F2">
         <v>5</v>
@@ -864,17 +871,17 @@
         <v>9</v>
       </c>
       <c r="C3">
-        <v>-1338.65</v>
+        <v>-1337.2</v>
       </c>
       <c r="D3">
-        <v>-1339.99</v>
+        <v>-1338.25</v>
       </c>
       <c r="E3" s="2">
         <f>-(C3-D3)/D3</f>
-        <v>1.0000074627421981E-3</v>
+        <v>7.8460676256301477E-4</v>
       </c>
       <c r="F3">
-        <v>194</v>
+        <v>3005</v>
       </c>
       <c r="G3" t="s">
         <v>13</v>
@@ -885,59 +892,207 @@
         <v>27</v>
       </c>
       <c r="C4">
-        <v>-1333.84</v>
+        <v>-1221.32</v>
       </c>
       <c r="D4">
-        <v>-1339.68</v>
+        <v>-1338.25</v>
       </c>
       <c r="E4" s="2">
         <f>-(C4-D4)/D4</f>
-        <v>4.3592499701422321E-3</v>
+        <v>8.7375303568092699E-2</v>
       </c>
       <c r="F4" s="5">
-        <v>20000</v>
+        <v>10000</v>
       </c>
       <c r="G4" t="s">
         <v>14</v>
       </c>
     </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6" t="s">
+        <v>0</v>
+      </c>
+      <c r="E6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B7">
+        <v>3</v>
+      </c>
+      <c r="C7" s="6">
+        <v>-1338.2470000000001</v>
+      </c>
+      <c r="D7" s="6">
+        <v>-1339.585</v>
+      </c>
+      <c r="E7" s="2">
+        <f>-(C7-D7)/D7</f>
+        <v>9.9881679773957256E-4</v>
+      </c>
+      <c r="F7">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B8">
+        <v>9</v>
+      </c>
+      <c r="C8" s="6">
+        <v>-1338.2470000000001</v>
+      </c>
+      <c r="D8" s="6">
+        <v>-1339.585</v>
+      </c>
+      <c r="E8" s="2">
+        <f>-(C8-D8)/D8</f>
+        <v>9.9881679773957256E-4</v>
+      </c>
+      <c r="F8">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B9">
+        <v>27</v>
+      </c>
+      <c r="C9" s="6">
+        <v>-1319.2560000000001</v>
+      </c>
+      <c r="D9" s="6">
+        <v>-1338.309</v>
+      </c>
+      <c r="E9" s="2">
+        <f>-(C9-D9)/D9</f>
+        <v>1.4236622484045077E-2</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" t="s">
+        <v>1</v>
+      </c>
+      <c r="D11" t="s">
+        <v>0</v>
+      </c>
+      <c r="E11" t="s">
+        <v>6</v>
+      </c>
+      <c r="F11" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B12">
+        <v>3</v>
+      </c>
+      <c r="C12" s="6">
+        <v>-1007.7889579159799</v>
+      </c>
+      <c r="D12" s="6">
+        <v>-2210.83461672973</v>
+      </c>
+      <c r="E12" s="2">
+        <f>-(C12-D12)/D12</f>
+        <v>0.54415904731639175</v>
+      </c>
+      <c r="F12" t="s">
+        <v>24</v>
+      </c>
+    </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+      <c r="B13">
+        <v>9</v>
+      </c>
+      <c r="C13" s="6">
+        <v>-1.3578666711118499E-6</v>
+      </c>
+      <c r="D13" s="6">
+        <v>-2390.5310000300201</v>
+      </c>
+      <c r="E13" s="2">
+        <f>-(C13-D13)/D13</f>
+        <v>0.99999999943198126</v>
+      </c>
+      <c r="F13" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B14">
+        <v>27</v>
+      </c>
+      <c r="C14" s="6">
+        <v>0</v>
+      </c>
+      <c r="D14" s="6">
+        <v>-2430.51977177764</v>
+      </c>
+      <c r="E14" s="2">
+        <f>-(C14-D14)/D14</f>
+        <v>1</v>
+      </c>
+      <c r="F14" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
         <v>10</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B21" t="s">
         <v>11</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C21" t="s">
         <v>18</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D21" t="s">
         <v>19</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E21" t="s">
         <v>16</v>
       </c>
-      <c r="F13" t="s">
+      <c r="F21" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22">
         <v>9</v>
       </c>
-      <c r="B14">
+      <c r="B22">
         <v>9</v>
       </c>
-      <c r="C14">
+      <c r="C22">
         <v>35</v>
       </c>
-      <c r="D14">
+      <c r="D22">
         <v>112</v>
       </c>
-      <c r="E14">
+      <c r="E22">
         <v>116</v>
       </c>
-      <c r="F14">
+      <c r="F22">
         <v>22</v>
       </c>
     </row>

</xml_diff>

<commit_message>
change the excel tables
</commit_message>
<xml_diff>
--- a/examples/PoolingContract/PoolingContract_results.xlsx
+++ b/examples/PoolingContract/PoolingContract_results.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26101"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28702"/>
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,15 +9,18 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="38940" yWindow="2240" windowWidth="27180" windowHeight="14440" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="39220" yWindow="500" windowWidth="36380" windowHeight="19100" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="branchAndBound" sheetId="2" r:id="rId1"/>
     <sheet name="DE" sheetId="3" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="4" r:id="rId3"/>
+    <sheet name="Presentation" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -26,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="53">
   <si>
     <t>LB</t>
   </si>
@@ -107,13 +110,100 @@
   </si>
   <si>
     <t>Solver=SCIP</t>
+  </si>
+  <si>
+    <t>#Scenarios</t>
+  </si>
+  <si>
+    <t>SCIP 5.0</t>
+  </si>
+  <si>
+    <t>BARON 18.5.8</t>
+  </si>
+  <si>
+    <t>ANTIGONE 1.1</t>
+  </si>
+  <si>
+    <t>5/0.1</t>
+  </si>
+  <si>
+    <t>3005/0.1</t>
+  </si>
+  <si>
+    <t>16/0.1</t>
+  </si>
+  <si>
+    <t>251/0.1</t>
+  </si>
+  <si>
+    <t>LD</t>
+  </si>
+  <si>
+    <t>walltime/gap</t>
+  </si>
+  <si>
+    <t>walltime/gap/#nodes</t>
+  </si>
+  <si>
+    <t>152/0.1
+1</t>
+  </si>
+  <si>
+    <t>502/0.1
+1</t>
+  </si>
+  <si>
+    <t>2113/0.1
+1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GBD(with cuts)+L </t>
+  </si>
+  <si>
+    <t>GBD+L</t>
+  </si>
+  <si>
+    <t>-/8.7</t>
+  </si>
+  <si>
+    <t>-/1.4</t>
+  </si>
+  <si>
+    <t>-/54.4</t>
+  </si>
+  <si>
+    <t>-/100.0</t>
+  </si>
+  <si>
+    <t>-/0.1
+381</t>
+  </si>
+  <si>
+    <t>-/0.8
+39</t>
+  </si>
+  <si>
+    <t>-/1.3
+7</t>
+  </si>
+  <si>
+    <t>-/0.2
+363</t>
+  </si>
+  <si>
+    <t>-/7.1
+43</t>
+  </si>
+  <si>
+    <t>-/12.2
+9</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -128,6 +218,28 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -137,7 +249,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -160,11 +272,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -172,8 +321,43 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="9">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -452,7 +636,7 @@
   <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -808,8 +992,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1103,12 +1287,143 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:L12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A1" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="7">
+        <v>3</v>
+      </c>
+      <c r="C1" s="7">
+        <v>9</v>
+      </c>
+      <c r="D1" s="7">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A3" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A4" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="H9" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="I9" s="7">
+        <v>3</v>
+      </c>
+      <c r="J9" s="7">
+        <v>9</v>
+      </c>
+      <c r="K9" s="7">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+      <c r="H10" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="I10" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="J10" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="K10" s="10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+      <c r="H11" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="I11" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="J11" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="K11" s="14" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="32" x14ac:dyDescent="0.2">
+      <c r="H12" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="I12" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="J12" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="K12" s="15" t="s">
+        <v>52</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>